<commit_message>
feat: baseline simulation in ClimateChangeRiskAssessment
Signed-off-by: yhHuang <qa4510qa@gmail.com>
</commit_message>
<xml_diff>
--- a/SDmodel/SD_inputData/Data_inflow.xlsx
+++ b/SDmodel/SD_inputData/Data_inflow.xlsx
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>5.345065473097614e-10</v>
+        <v>6.487708416141559e-07</v>
       </c>
       <c r="D2" t="n">
         <v>1000000</v>
@@ -479,7 +479,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>9.743187412166676e-12</v>
+        <v>1.182604016585146e-08</v>
       </c>
       <c r="D3" t="n">
         <v>1000001</v>
@@ -497,7 +497,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="n">
-        <v>1.786906831062936e-13</v>
+        <v>46751564.37907436</v>
       </c>
       <c r="D4" t="n">
         <v>1000002</v>
@@ -515,7 +515,7 @@
         <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>2.169061735882321e-15</v>
+        <v>843412.7080118682</v>
       </c>
       <c r="D5" t="n">
         <v>1000003</v>
@@ -533,7 +533,7 @@
         <v>42</v>
       </c>
       <c r="C6" t="n">
-        <v>3.953847732572962e-17</v>
+        <v>116494.0962686534</v>
       </c>
       <c r="D6" t="n">
         <v>1000004</v>
@@ -551,7 +551,7 @@
         <v>52</v>
       </c>
       <c r="C7" t="n">
-        <v>7.042942503469e-19</v>
+        <v>24111650.68432828</v>
       </c>
       <c r="D7" t="n">
         <v>1000005</v>
@@ -569,7 +569,7 @@
         <v>60</v>
       </c>
       <c r="C8" t="n">
-        <v>2.926620354123306e-20</v>
+        <v>11335933.31210752</v>
       </c>
       <c r="D8" t="n">
         <v>1000006</v>
@@ -587,7 +587,7 @@
         <v>70</v>
       </c>
       <c r="C9" t="n">
-        <v>275339468.6111208</v>
+        <v>13681675.36496993</v>
       </c>
       <c r="D9" t="n">
         <v>1000007</v>
@@ -605,7 +605,7 @@
         <v>80</v>
       </c>
       <c r="C10" t="n">
-        <v>242248755.20175</v>
+        <v>960689.5850188414</v>
       </c>
       <c r="D10" t="n">
         <v>1000008</v>
@@ -623,7 +623,7 @@
         <v>91</v>
       </c>
       <c r="C11" t="n">
-        <v>8389567.147887185</v>
+        <v>60168433.01643151</v>
       </c>
       <c r="D11" t="n">
         <v>1000009</v>
@@ -641,7 +641,7 @@
         <v>101</v>
       </c>
       <c r="C12" t="n">
-        <v>14665398.09033637</v>
+        <v>22019306.84109979</v>
       </c>
       <c r="D12" t="n">
         <v>1000010</v>
@@ -659,7 +659,7 @@
         <v>111</v>
       </c>
       <c r="C13" t="n">
-        <v>392294.3970124396</v>
+        <v>401376.2493998191</v>
       </c>
       <c r="D13" t="n">
         <v>1000011</v>
@@ -677,7 +677,7 @@
         <v>121</v>
       </c>
       <c r="C14" t="n">
-        <v>24314916.00705337</v>
+        <v>31278054.07264849</v>
       </c>
       <c r="D14" t="n">
         <v>1000012</v>
@@ -695,7 +695,7 @@
         <v>131</v>
       </c>
       <c r="C15" t="n">
-        <v>15533455.31392152</v>
+        <v>3757594.980442458</v>
       </c>
       <c r="D15" t="n">
         <v>1000013</v>
@@ -713,7 +713,7 @@
         <v>141</v>
       </c>
       <c r="C16" t="n">
-        <v>289456.692219872</v>
+        <v>32595011.41656321</v>
       </c>
       <c r="D16" t="n">
         <v>1000014</v>
@@ -731,7 +731,7 @@
         <v>152</v>
       </c>
       <c r="C17" t="n">
-        <v>13650173.9885916</v>
+        <v>107439536.1809415</v>
       </c>
       <c r="D17" t="n">
         <v>1000015</v>
@@ -749,7 +749,7 @@
         <v>162</v>
       </c>
       <c r="C18" t="n">
-        <v>100148006.3807181</v>
+        <v>53743950.33948664</v>
       </c>
       <c r="D18" t="n">
         <v>1000016</v>
@@ -767,7 +767,7 @@
         <v>172</v>
       </c>
       <c r="C19" t="n">
-        <v>36186141.50983578</v>
+        <v>73130376.27633405</v>
       </c>
       <c r="D19" t="n">
         <v>1000017</v>
@@ -785,7 +785,7 @@
         <v>182</v>
       </c>
       <c r="C20" t="n">
-        <v>6917830.911737612</v>
+        <v>21142893.90270996</v>
       </c>
       <c r="D20" t="n">
         <v>1000018</v>
@@ -803,7 +803,7 @@
         <v>192</v>
       </c>
       <c r="C21" t="n">
-        <v>253147.5721635911</v>
+        <v>385400.6630348664</v>
       </c>
       <c r="D21" t="n">
         <v>1000019</v>
@@ -821,7 +821,7 @@
         <v>202</v>
       </c>
       <c r="C22" t="n">
-        <v>4642.742737363862</v>
+        <v>27657845.60669194</v>
       </c>
       <c r="D22" t="n">
         <v>1000020</v>
@@ -839,7 +839,7 @@
         <v>213</v>
       </c>
       <c r="C23" t="n">
-        <v>56.35657912377646</v>
+        <v>15305410.29521715</v>
       </c>
       <c r="D23" t="n">
         <v>1000021</v>
@@ -857,7 +857,7 @@
         <v>223</v>
       </c>
       <c r="C24" t="n">
-        <v>1.027289029620323</v>
+        <v>18763263.71127747</v>
       </c>
       <c r="D24" t="n">
         <v>1000022</v>
@@ -875,7 +875,7 @@
         <v>233</v>
       </c>
       <c r="C25" t="n">
-        <v>8325387.684332496</v>
+        <v>1255195.668910339</v>
       </c>
       <c r="D25" t="n">
         <v>1000023</v>
@@ -893,7 +893,7 @@
         <v>244</v>
       </c>
       <c r="C26" t="n">
-        <v>32240204.35755538</v>
+        <v>15236.36738720788</v>
       </c>
       <c r="D26" t="n">
         <v>1000024</v>
@@ -911,7 +911,7 @@
         <v>254</v>
       </c>
       <c r="C27" t="n">
-        <v>136921576.7191159</v>
+        <v>277.7342647744208</v>
       </c>
       <c r="D27" t="n">
         <v>1000025</v>
@@ -929,7 +929,7 @@
         <v>264</v>
       </c>
       <c r="C28" t="n">
-        <v>467264292.8254446</v>
+        <v>176884907.5101677</v>
       </c>
       <c r="D28" t="n">
         <v>1000026</v>
@@ -947,7 +947,7 @@
         <v>274</v>
       </c>
       <c r="C29" t="n">
-        <v>90595662.6965982</v>
+        <v>12382544.41762704</v>
       </c>
       <c r="D29" t="n">
         <v>1000027</v>
@@ -965,7 +965,7 @@
         <v>284</v>
       </c>
       <c r="C30" t="n">
-        <v>113413027.5102438</v>
+        <v>225713.7008099194</v>
       </c>
       <c r="D30" t="n">
         <v>1000028</v>
@@ -983,7 +983,7 @@
         <v>294</v>
       </c>
       <c r="C31" t="n">
-        <v>19697213.87665647</v>
+        <v>4139.603774203179</v>
       </c>
       <c r="D31" t="n">
         <v>1000029</v>
@@ -1001,7 +1001,7 @@
         <v>305</v>
       </c>
       <c r="C32" t="n">
-        <v>239097.3730730622</v>
+        <v>50.2491567677146</v>
       </c>
       <c r="D32" t="n">
         <v>1000030</v>
@@ -1019,7 +1019,7 @@
         <v>315</v>
       </c>
       <c r="C33" t="n">
-        <v>4358.35730606594</v>
+        <v>0.9159606260303816</v>
       </c>
       <c r="D33" t="n">
         <v>1000031</v>
@@ -1037,7 +1037,7 @@
         <v>325</v>
       </c>
       <c r="C34" t="n">
-        <v>79.44578463241365</v>
+        <v>0.01669647656609077</v>
       </c>
       <c r="D34" t="n">
         <v>1000032</v>
@@ -1055,7 +1055,7 @@
         <v>335</v>
       </c>
       <c r="C35" t="n">
-        <v>1.44816779640241</v>
+        <v>0.0003043496868748282</v>
       </c>
       <c r="D35" t="n">
         <v>1000033</v>
@@ -1073,7 +1073,7 @@
         <v>345</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0263977500661673</v>
+        <v>5.547801150389279e-06</v>
       </c>
       <c r="D36" t="n">
         <v>1000034</v>
@@ -1091,7 +1091,7 @@
         <v>355</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0004841364321805316</v>
+        <v>1.017470295257811e-07</v>
       </c>
       <c r="D37" t="n">
         <v>1000035</v>

</xml_diff>

<commit_message>
feat: fix discharge estimation error in SDmodel inputfile reading
Signed-off-by: yhHuang <qa4510qa@gmail.com>
</commit_message>
<xml_diff>
--- a/SDmodel/SD_inputData/Data_inflow.xlsx
+++ b/SDmodel/SD_inputData/Data_inflow.xlsx
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>6.487708416141559e-07</v>
+        <v>3.851225878354915e-10</v>
       </c>
       <c r="D2" t="n">
         <v>1000000</v>
@@ -479,7 +479,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>1.182604016585146e-08</v>
+        <v>7.020160124933402e-12</v>
       </c>
       <c r="D3" t="n">
         <v>1000001</v>
@@ -497,7 +497,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="n">
-        <v>46751564.37907436</v>
+        <v>1.170456251936844e-13</v>
       </c>
       <c r="D4" t="n">
         <v>1000002</v>
@@ -515,7 +515,7 @@
         <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>843412.7080118682</v>
+        <v>1.562852079366264e-15</v>
       </c>
       <c r="D5" t="n">
         <v>1000003</v>
@@ -533,7 +533,7 @@
         <v>42</v>
       </c>
       <c r="C6" t="n">
-        <v>116494.0962686534</v>
+        <v>2.848825853191154e-17</v>
       </c>
       <c r="D6" t="n">
         <v>1000004</v>
@@ -551,7 +551,7 @@
         <v>52</v>
       </c>
       <c r="C7" t="n">
-        <v>24111650.68432828</v>
+        <v>6.343225018861762e-19</v>
       </c>
       <c r="D7" t="n">
         <v>1000005</v>
@@ -569,7 +569,7 @@
         <v>60</v>
       </c>
       <c r="C8" t="n">
-        <v>11335933.31210752</v>
+        <v>2.108688116291305e-20</v>
       </c>
       <c r="D8" t="n">
         <v>1000006</v>
@@ -587,7 +587,7 @@
         <v>70</v>
       </c>
       <c r="C9" t="n">
-        <v>13681675.36496993</v>
+        <v>3.843796416384833e-22</v>
       </c>
       <c r="D9" t="n">
         <v>1000007</v>
@@ -605,7 +605,7 @@
         <v>80</v>
       </c>
       <c r="C10" t="n">
-        <v>960689.5850188414</v>
+        <v>6.408679384322087e-24</v>
       </c>
       <c r="D10" t="n">
         <v>1000008</v>
@@ -623,7 +623,7 @@
         <v>91</v>
       </c>
       <c r="C11" t="n">
-        <v>60168433.01643151</v>
+        <v>134962.5154844009</v>
       </c>
       <c r="D11" t="n">
         <v>1000009</v>
@@ -641,7 +641,7 @@
         <v>101</v>
       </c>
       <c r="C12" t="n">
-        <v>22019306.84109979</v>
+        <v>1757832.594709143</v>
       </c>
       <c r="D12" t="n">
         <v>1000010</v>
@@ -659,7 +659,7 @@
         <v>111</v>
       </c>
       <c r="C13" t="n">
-        <v>401376.2493998191</v>
+        <v>768538.6203265248</v>
       </c>
       <c r="D13" t="n">
         <v>1000011</v>
@@ -677,7 +677,7 @@
         <v>121</v>
       </c>
       <c r="C14" t="n">
-        <v>31278054.07264849</v>
+        <v>974563.6817176824</v>
       </c>
       <c r="D14" t="n">
         <v>1000012</v>
@@ -695,7 +695,7 @@
         <v>131</v>
       </c>
       <c r="C15" t="n">
-        <v>3757594.980442458</v>
+        <v>452613.5335914007</v>
       </c>
       <c r="D15" t="n">
         <v>1000013</v>
@@ -713,7 +713,7 @@
         <v>141</v>
       </c>
       <c r="C16" t="n">
-        <v>32595011.41656321</v>
+        <v>26198.84397427095</v>
       </c>
       <c r="D16" t="n">
         <v>1000014</v>
@@ -731,7 +731,7 @@
         <v>152</v>
       </c>
       <c r="C17" t="n">
-        <v>107439536.1809415</v>
+        <v>16269835.90682306</v>
       </c>
       <c r="D17" t="n">
         <v>1000015</v>
@@ -749,7 +749,7 @@
         <v>162</v>
       </c>
       <c r="C18" t="n">
-        <v>53743950.33948664</v>
+        <v>15702821.79366891</v>
       </c>
       <c r="D18" t="n">
         <v>1000016</v>
@@ -767,7 +767,7 @@
         <v>172</v>
       </c>
       <c r="C19" t="n">
-        <v>73130376.27633405</v>
+        <v>8331903.210997708</v>
       </c>
       <c r="D19" t="n">
         <v>1000017</v>
@@ -785,7 +785,7 @@
         <v>182</v>
       </c>
       <c r="C20" t="n">
-        <v>21142893.90270996</v>
+        <v>7629416.52609037</v>
       </c>
       <c r="D20" t="n">
         <v>1000018</v>
@@ -803,7 +803,7 @@
         <v>192</v>
       </c>
       <c r="C21" t="n">
-        <v>385400.6630348664</v>
+        <v>4304435.526403553</v>
       </c>
       <c r="D21" t="n">
         <v>1000019</v>
@@ -821,7 +821,7 @@
         <v>202</v>
       </c>
       <c r="C22" t="n">
-        <v>27657845.60669194</v>
+        <v>1612123.061485417</v>
       </c>
       <c r="D22" t="n">
         <v>1000020</v>
@@ -839,7 +839,7 @@
         <v>213</v>
       </c>
       <c r="C23" t="n">
-        <v>15305410.29521715</v>
+        <v>1124896.296864709</v>
       </c>
       <c r="D23" t="n">
         <v>1000021</v>
@@ -857,7 +857,7 @@
         <v>223</v>
       </c>
       <c r="C24" t="n">
-        <v>18763263.71127747</v>
+        <v>2849689.676257911</v>
       </c>
       <c r="D24" t="n">
         <v>1000022</v>
@@ -875,7 +875,7 @@
         <v>233</v>
       </c>
       <c r="C25" t="n">
-        <v>1255195.668910339</v>
+        <v>788393.6281928831</v>
       </c>
       <c r="D25" t="n">
         <v>1000023</v>
@@ -893,7 +893,7 @@
         <v>244</v>
       </c>
       <c r="C26" t="n">
-        <v>15236.36738720788</v>
+        <v>4987356.099866037</v>
       </c>
       <c r="D26" t="n">
         <v>1000024</v>
@@ -911,7 +911,7 @@
         <v>254</v>
       </c>
       <c r="C27" t="n">
-        <v>277.7342647744208</v>
+        <v>10834204.15497985</v>
       </c>
       <c r="D27" t="n">
         <v>1000025</v>
@@ -929,7 +929,7 @@
         <v>264</v>
       </c>
       <c r="C28" t="n">
-        <v>176884907.5101677</v>
+        <v>348766.2390630613</v>
       </c>
       <c r="D28" t="n">
         <v>1000026</v>
@@ -947,7 +947,7 @@
         <v>274</v>
       </c>
       <c r="C29" t="n">
-        <v>12382544.41762704</v>
+        <v>6357.442855154855</v>
       </c>
       <c r="D29" t="n">
         <v>1000027</v>
@@ -965,7 +965,7 @@
         <v>284</v>
       </c>
       <c r="C30" t="n">
-        <v>225713.7008099194</v>
+        <v>115.8858717665375</v>
       </c>
       <c r="D30" t="n">
         <v>1000028</v>
@@ -983,7 +983,7 @@
         <v>294</v>
       </c>
       <c r="C31" t="n">
-        <v>4139.603774203179</v>
+        <v>1.932140303161275</v>
       </c>
       <c r="D31" t="n">
         <v>1000029</v>
@@ -1001,7 +1001,7 @@
         <v>305</v>
       </c>
       <c r="C32" t="n">
-        <v>50.2491567677146</v>
+        <v>0.02579890948872387</v>
       </c>
       <c r="D32" t="n">
         <v>1000030</v>
@@ -1019,7 +1019,7 @@
         <v>315</v>
       </c>
       <c r="C33" t="n">
-        <v>0.9159606260303816</v>
+        <v>243074.544019867</v>
       </c>
       <c r="D33" t="n">
         <v>1000031</v>
@@ -1037,7 +1037,7 @@
         <v>325</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01669647656609077</v>
+        <v>484519.0046972869</v>
       </c>
       <c r="D34" t="n">
         <v>1000032</v>
@@ -1055,7 +1055,7 @@
         <v>335</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0003043496868748282</v>
+        <v>8831.995587860069</v>
       </c>
       <c r="D35" t="n">
         <v>1000033</v>
@@ -1073,7 +1073,7 @@
         <v>345</v>
       </c>
       <c r="C36" t="n">
-        <v>5.547801150389279e-06</v>
+        <v>160.9929544718569</v>
       </c>
       <c r="D36" t="n">
         <v>1000034</v>
@@ -1091,7 +1091,7 @@
         <v>355</v>
       </c>
       <c r="C37" t="n">
-        <v>1.017470295257811e-07</v>
+        <v>2.684201025701763</v>
       </c>
       <c r="D37" t="n">
         <v>1000035</v>

</xml_diff>

<commit_message>
feat: finish all subModel validation
Signed-off-by: yhHuang <qa4510qa@gmail.com>
</commit_message>
<xml_diff>
--- a/SDmodel/SD_inputData/Data_inflow.xlsx
+++ b/SDmodel/SD_inputData/Data_inflow.xlsx
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>3.851225878354915e-10</v>
+        <v>2.673464068582278e-10</v>
       </c>
       <c r="D2" t="n">
         <v>1000000</v>
@@ -479,7 +479,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>7.020160124933402e-12</v>
+        <v>4.873291373322538e-12</v>
       </c>
       <c r="D3" t="n">
         <v>1000001</v>
@@ -497,7 +497,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="n">
-        <v>1.170456251936844e-13</v>
+        <v>8.125134261762103e-14</v>
       </c>
       <c r="D4" t="n">
         <v>1000002</v>
@@ -515,7 +515,7 @@
         <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>1.562852079366264e-15</v>
+        <v>1.084908808433633e-15</v>
       </c>
       <c r="D5" t="n">
         <v>1000003</v>
@@ -533,7 +533,7 @@
         <v>42</v>
       </c>
       <c r="C6" t="n">
-        <v>2.848825853191154e-17</v>
+        <v>1.97761279050403e-17</v>
       </c>
       <c r="D6" t="n">
         <v>1000004</v>
@@ -551,7 +551,7 @@
         <v>52</v>
       </c>
       <c r="C7" t="n">
-        <v>6.343225018861762e-19</v>
+        <v>4.403373030434395e-19</v>
       </c>
       <c r="D7" t="n">
         <v>1000005</v>
@@ -569,7 +569,7 @@
         <v>60</v>
       </c>
       <c r="C8" t="n">
-        <v>2.108688116291305e-20</v>
+        <v>1.463820115676871e-20</v>
       </c>
       <c r="D8" t="n">
         <v>1000006</v>
@@ -587,7 +587,7 @@
         <v>70</v>
       </c>
       <c r="C9" t="n">
-        <v>3.843796416384833e-22</v>
+        <v>2.668306645919132e-22</v>
       </c>
       <c r="D9" t="n">
         <v>1000007</v>
@@ -605,7 +605,7 @@
         <v>80</v>
       </c>
       <c r="C10" t="n">
-        <v>6.408679384322087e-24</v>
+        <v>28737605.28126813</v>
       </c>
       <c r="D10" t="n">
         <v>1000008</v>
@@ -623,7 +623,7 @@
         <v>91</v>
       </c>
       <c r="C11" t="n">
-        <v>134962.5154844009</v>
+        <v>47367919.11726144</v>
       </c>
       <c r="D11" t="n">
         <v>1000009</v>
@@ -641,7 +641,7 @@
         <v>101</v>
       </c>
       <c r="C12" t="n">
-        <v>1757832.594709143</v>
+        <v>6198942.399057668</v>
       </c>
       <c r="D12" t="n">
         <v>1000010</v>
@@ -659,7 +659,7 @@
         <v>111</v>
       </c>
       <c r="C13" t="n">
-        <v>768538.6203265248</v>
+        <v>606720.050152338</v>
       </c>
       <c r="D13" t="n">
         <v>1000011</v>
@@ -677,7 +677,7 @@
         <v>121</v>
       </c>
       <c r="C14" t="n">
-        <v>974563.6817176824</v>
+        <v>381265.2628932028</v>
       </c>
       <c r="D14" t="n">
         <v>1000012</v>
@@ -695,7 +695,7 @@
         <v>131</v>
       </c>
       <c r="C15" t="n">
-        <v>452613.5335914007</v>
+        <v>1843598.123654923</v>
       </c>
       <c r="D15" t="n">
         <v>1000013</v>
@@ -713,7 +713,7 @@
         <v>141</v>
       </c>
       <c r="C16" t="n">
-        <v>26198.84397427095</v>
+        <v>3989157.845993724</v>
       </c>
       <c r="D16" t="n">
         <v>1000014</v>
@@ -731,7 +731,7 @@
         <v>152</v>
       </c>
       <c r="C17" t="n">
-        <v>16269835.90682306</v>
+        <v>1468310.73679977</v>
       </c>
       <c r="D17" t="n">
         <v>1000015</v>
@@ -749,7 +749,7 @@
         <v>162</v>
       </c>
       <c r="C18" t="n">
-        <v>15702821.79366891</v>
+        <v>5093586.178880416</v>
       </c>
       <c r="D18" t="n">
         <v>1000016</v>
@@ -767,7 +767,7 @@
         <v>172</v>
       </c>
       <c r="C19" t="n">
-        <v>8331903.210997708</v>
+        <v>3895831.753260836</v>
       </c>
       <c r="D19" t="n">
         <v>1000017</v>
@@ -785,7 +785,7 @@
         <v>182</v>
       </c>
       <c r="C20" t="n">
-        <v>7629416.52609037</v>
+        <v>1464907.003552919</v>
       </c>
       <c r="D20" t="n">
         <v>1000018</v>
@@ -803,7 +803,7 @@
         <v>192</v>
       </c>
       <c r="C21" t="n">
-        <v>4304435.526403553</v>
+        <v>823116.3961698734</v>
       </c>
       <c r="D21" t="n">
         <v>1000019</v>
@@ -821,7 +821,7 @@
         <v>202</v>
       </c>
       <c r="C22" t="n">
-        <v>1612123.061485417</v>
+        <v>27666753.56719804</v>
       </c>
       <c r="D22" t="n">
         <v>1000020</v>
@@ -839,7 +839,7 @@
         <v>213</v>
       </c>
       <c r="C23" t="n">
-        <v>1124896.296864709</v>
+        <v>15533351.07477352</v>
       </c>
       <c r="D23" t="n">
         <v>1000021</v>
@@ -857,7 +857,7 @@
         <v>223</v>
       </c>
       <c r="C24" t="n">
-        <v>2849689.676257911</v>
+        <v>10470277.57532721</v>
       </c>
       <c r="D24" t="n">
         <v>1000022</v>
@@ -875,7 +875,7 @@
         <v>233</v>
       </c>
       <c r="C25" t="n">
-        <v>788393.6281928831</v>
+        <v>30054754.88219407</v>
       </c>
       <c r="D25" t="n">
         <v>1000023</v>
@@ -893,7 +893,7 @@
         <v>244</v>
       </c>
       <c r="C26" t="n">
-        <v>4987356.099866037</v>
+        <v>43284961.16163335</v>
       </c>
       <c r="D26" t="n">
         <v>1000024</v>
@@ -911,7 +911,7 @@
         <v>254</v>
       </c>
       <c r="C27" t="n">
-        <v>10834204.15497985</v>
+        <v>1539754.277264587</v>
       </c>
       <c r="D27" t="n">
         <v>1000025</v>
@@ -929,7 +929,7 @@
         <v>264</v>
       </c>
       <c r="C28" t="n">
-        <v>348766.2390630613</v>
+        <v>28067.22306318163</v>
       </c>
       <c r="D28" t="n">
         <v>1000026</v>
@@ -947,7 +947,7 @@
         <v>274</v>
       </c>
       <c r="C29" t="n">
-        <v>6357.442855154855</v>
+        <v>3898539.119242128</v>
       </c>
       <c r="D29" t="n">
         <v>1000027</v>
@@ -965,7 +965,7 @@
         <v>284</v>
       </c>
       <c r="C30" t="n">
-        <v>115.8858717665375</v>
+        <v>901721.1200063666</v>
       </c>
       <c r="D30" t="n">
         <v>1000028</v>
@@ -983,7 +983,7 @@
         <v>294</v>
       </c>
       <c r="C31" t="n">
-        <v>1.932140303161275</v>
+        <v>15034.20297588949</v>
       </c>
       <c r="D31" t="n">
         <v>1000029</v>
@@ -1001,7 +1001,7 @@
         <v>305</v>
       </c>
       <c r="C32" t="n">
-        <v>0.02579890948872387</v>
+        <v>200.7442426284821</v>
       </c>
       <c r="D32" t="n">
         <v>1000030</v>
@@ -1019,7 +1019,7 @@
         <v>315</v>
       </c>
       <c r="C33" t="n">
-        <v>243074.544019867</v>
+        <v>3.659241945093084</v>
       </c>
       <c r="D33" t="n">
         <v>1000031</v>
@@ -1037,7 +1037,7 @@
         <v>325</v>
       </c>
       <c r="C34" t="n">
-        <v>484519.0046972869</v>
+        <v>0.06670204553517191</v>
       </c>
       <c r="D34" t="n">
         <v>1000032</v>
@@ -1055,7 +1055,7 @@
         <v>335</v>
       </c>
       <c r="C35" t="n">
-        <v>8831.995587860069</v>
+        <v>0.001215870102424443</v>
       </c>
       <c r="D35" t="n">
         <v>1000033</v>
@@ -1073,7 +1073,7 @@
         <v>345</v>
       </c>
       <c r="C36" t="n">
-        <v>160.9929544718569</v>
+        <v>291937.8988855762</v>
       </c>
       <c r="D36" t="n">
         <v>1000034</v>
@@ -1091,7 +1091,7 @@
         <v>355</v>
       </c>
       <c r="C37" t="n">
-        <v>2.684201025701763</v>
+        <v>75648.12973465728</v>
       </c>
       <c r="D37" t="n">
         <v>1000035</v>

</xml_diff>